<commit_message>
Cleaned up the data processing
You now have complete control over what operation is called.

It is now possible to generate the metadata from a dataset.
</commit_message>
<xml_diff>
--- a/examples/Australia OGD/coloured labour/counters_summary.xlsx
+++ b/examples/Australia OGD/coloured labour/counters_summary.xlsx
@@ -469,7 +469,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>0.001</v>
+        <v>0.001199</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -532,7 +532,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>0.0009</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -666,7 +666,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.001</v>
+        <v>0.001199</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -690,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>0.0003</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -733,7 +733,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001</v>
+        <v>0.001199</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
@@ -757,7 +757,7 @@
         <v>24</v>
       </c>
       <c r="K6" t="n">
-        <v>0.004</v>
+        <v>0.007196</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>0.001</v>
+        <v>0.001199</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -867,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.0009</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -891,7 +891,7 @@
         <v>325</v>
       </c>
       <c r="K8" t="n">
-        <v>0.049</v>
+        <v>0.097451</v>
       </c>
       <c r="L8" t="n">
         <v>0</v>
@@ -934,7 +934,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>0.001</v>
+        <v>0.001199</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
@@ -1001,7 +1001,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>0.001</v>
+        <v>0.001499</v>
       </c>
       <c r="D10" t="n">
         <v>0</v>
@@ -1068,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="C11" t="n">
-        <v>0.001</v>
+        <v>0.001199</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>

</xml_diff>